<commit_message>
Guang Dong Zhu Ready for online
Horray.
Fei Yu still GGYY.
</commit_message>
<xml_diff>
--- a/Attach/FactoryClient/FactoryClient/bin/Debug/精緻化報表.xlsx
+++ b/Attach/FactoryClient/FactoryClient/bin/Debug/精緻化報表.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21328"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE07DE06-2A62-4F4D-920C-6C8542BFF197}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -14,39 +15,33 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>點單號</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>素</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <t>點餐者</t>
   </si>
   <si>
-    <t>香</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>大雞排</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <t>時間</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -76,7 +71,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="一般" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="1">
     <dxf>
@@ -111,7 +106,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 佈景主題">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -186,6 +181,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -221,6 +233,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -396,16 +425,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R7" sqref="R7"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
+  <cols>
+    <col min="2" max="2" width="14.75" customWidth="1"/>
+    <col min="3" max="3" width="21.5" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -414,9 +447,6 @@
       </c>
       <c r="C1" t="s">
         <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Factory cleint UI fix
</commit_message>
<xml_diff>
--- a/Attach/FactoryClient/FactoryClient/bin/Debug/精緻化報表.xlsx
+++ b/Attach/FactoryClient/FactoryClient/bin/Debug/精緻化報表.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21328"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE07DE06-2A62-4F4D-920C-6C8542BFF197}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD71E64A-67C1-40F2-810C-8CA8CAE9D894}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6060" yWindow="2610" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>點單號</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -25,6 +25,93 @@
   </si>
   <si>
     <t>時間</t>
+  </si>
+  <si>
+    <t>總價</t>
+  </si>
+  <si>
+    <t>冬粉</t>
+  </si>
+  <si>
+    <t>烏龍麵</t>
+  </si>
+  <si>
+    <t>鍋燒麵</t>
+  </si>
+  <si>
+    <t>肉片</t>
+  </si>
+  <si>
+    <t>貢丸</t>
+  </si>
+  <si>
+    <t>龍蝦丸</t>
+  </si>
+  <si>
+    <t>黃金魚蛋</t>
+  </si>
+  <si>
+    <t>魚豆腐</t>
+  </si>
+  <si>
+    <t>起司丸</t>
+  </si>
+  <si>
+    <t>鱈魚丸</t>
+  </si>
+  <si>
+    <t>菜頭</t>
+  </si>
+  <si>
+    <t>百頁豆腐</t>
+  </si>
+  <si>
+    <t>豬血糕</t>
+  </si>
+  <si>
+    <t>油豆腐</t>
+  </si>
+  <si>
+    <t>甜不辣</t>
+  </si>
+  <si>
+    <t>竹輪</t>
+  </si>
+  <si>
+    <t>黑輪</t>
+  </si>
+  <si>
+    <t>杏孢菇</t>
+  </si>
+  <si>
+    <t>金針菇</t>
+  </si>
+  <si>
+    <t>鑫鑫腸</t>
+  </si>
+  <si>
+    <t>滷蛋</t>
+  </si>
+  <si>
+    <t>馬鈴薯</t>
+  </si>
+  <si>
+    <t>豆皮</t>
+  </si>
+  <si>
+    <t>魚餃</t>
+  </si>
+  <si>
+    <t>餛飩</t>
+  </si>
+  <si>
+    <t>年糕</t>
+  </si>
+  <si>
+    <t>玉米筍</t>
+  </si>
+  <si>
+    <t>高麗菜</t>
   </si>
 </sst>
 </file>
@@ -55,7 +142,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -63,12 +150,34 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -426,32 +535,384 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:AF10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="3.625" defaultRowHeight="15.75"/>
   <cols>
-    <col min="2" max="2" width="14.75" customWidth="1"/>
-    <col min="3" max="3" width="21.5" customWidth="1"/>
+    <col min="1" max="1" width="9" customWidth="1"/>
+    <col min="2" max="2" width="9.125" customWidth="1"/>
+    <col min="3" max="3" width="8.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:32" s="2" customFormat="1" ht="92.25" customHeight="1">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="AF1" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:32">
+      <c r="A2">
+        <v>41111</v>
+      </c>
+      <c r="B2">
+        <v>21724</v>
+      </c>
+      <c r="C2" s="3">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="D2">
+        <v>60</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="AA2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:32">
+      <c r="A3">
+        <v>41120</v>
+      </c>
+      <c r="B3">
+        <v>10717</v>
+      </c>
+      <c r="C3" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="D3">
+        <v>60</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="AA3">
+        <v>1</v>
+      </c>
+      <c r="AC3">
+        <v>1</v>
+      </c>
+      <c r="AF3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:32">
+      <c r="A4">
+        <v>41124</v>
+      </c>
+      <c r="B4">
+        <v>11506</v>
+      </c>
+      <c r="C4" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="D4">
+        <v>50</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="P4">
+        <v>1</v>
+      </c>
+      <c r="Y4">
+        <v>1</v>
+      </c>
+      <c r="AF4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:32">
+      <c r="A5">
+        <v>41172</v>
+      </c>
+      <c r="B5">
+        <v>10316</v>
+      </c>
+      <c r="C5" s="3">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="D5">
+        <v>60</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="V5">
+        <v>1</v>
+      </c>
+      <c r="X5">
+        <v>1</v>
+      </c>
+      <c r="AA5">
+        <v>1</v>
+      </c>
+      <c r="AE5">
+        <v>1</v>
+      </c>
+      <c r="AF5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:32">
+      <c r="A6">
+        <v>41176</v>
+      </c>
+      <c r="B6">
+        <v>10415</v>
+      </c>
+      <c r="C6" s="3">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="D6">
+        <v>75</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="M6">
+        <v>1</v>
+      </c>
+      <c r="R6">
+        <v>1</v>
+      </c>
+      <c r="W6">
+        <v>1</v>
+      </c>
+      <c r="AF6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:32">
+      <c r="A7">
+        <v>41210</v>
+      </c>
+      <c r="B7">
+        <v>21109</v>
+      </c>
+      <c r="C7" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="D7">
+        <v>60</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="Q7">
+        <v>1</v>
+      </c>
+      <c r="R7">
+        <v>1</v>
+      </c>
+      <c r="Y7">
+        <v>1</v>
+      </c>
+      <c r="AA7">
+        <v>1</v>
+      </c>
+      <c r="AF7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:32">
+      <c r="A8">
+        <v>41211</v>
+      </c>
+      <c r="B8">
+        <v>21130</v>
+      </c>
+      <c r="C8" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="D8">
+        <v>50</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="Y8">
+        <v>1</v>
+      </c>
+      <c r="AF8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:32">
+      <c r="A9">
+        <v>41212</v>
+      </c>
+      <c r="B9">
+        <v>11601</v>
+      </c>
+      <c r="C9" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="D9">
+        <v>60</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="H9">
+        <v>1</v>
+      </c>
+      <c r="X9">
+        <v>1</v>
+      </c>
+      <c r="AA9">
+        <v>1</v>
+      </c>
+      <c r="AE9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:32">
+      <c r="A10">
+        <v>41248</v>
+      </c>
+      <c r="B10">
+        <v>21005</v>
+      </c>
+      <c r="C10" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="D10">
+        <v>75</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="H10">
+        <v>1</v>
+      </c>
+      <c r="I10">
+        <v>1</v>
+      </c>
+      <c r="P10">
+        <v>1</v>
+      </c>
+      <c r="AE10">
+        <v>1</v>
+      </c>
+      <c r="AF10">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="A2:P10000">
+  <conditionalFormatting sqref="A2:ZZ10000">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>AND($A2=INT($A2),NOT($A2=""))</formula>
     </cfRule>

</xml_diff>